<commit_message>
Baseboard_v0106 1)Fix D-0020567 --- <EVT FW BB CPLD> Register 80h 0b/1b is reversed to reflect the low active signal. 2)Fix D-0020797 --- <EVT FW BB CPLD> BB CPLD1/2 couldn't be reset by BB_CPLD1/2_RST_L signal.
</commit_message>
<xml_diff>
--- a/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
+++ b/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
-  <si>
-    <t>D-0020567</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>0-None</t>
   </si>
@@ -27,15 +24,6 @@
     <t>Assigned</t>
   </si>
   <si>
-    <t>&lt;EVT FW BB CPLD&gt; Register 80h 0b/1b is reversed to reflect the low active signal.</t>
-  </si>
-  <si>
-    <t>D-0020797</t>
-  </si>
-  <si>
-    <t>&lt;EVT FW BB CPLD&gt; BB CPLD1/2 couldn't be reset by BB_CPLD1/2_RST_L signal.</t>
-  </si>
-  <si>
     <t>D-0020536</t>
   </si>
   <si>
@@ -82,52 +70,6 @@
   </si>
   <si>
     <t>&lt;EVT FW BB CPLD&gt; Defalut value of some regsiters are not compliant with desgin spec</t>
-  </si>
-  <si>
-    <t>[Hardware] 
-Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
-Midplane - P/N: PBA001528A-A03, SN: JD37140690 
-BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
-[SW/FW Ver: Package 1] 
-Controller CPLD: V01.08 
-MI CPLD: V01.03 
-SXP: 0110[3257] 
-BMC: V005 
-Bios: V0101 
-BB CPLD: V01.02 
-SSM CPLD: V01.01 
-[Description] 
-MI CPLD register 40h BB_CPLD1/2_RST is required to drive BB_CPLD1/2_RST_L signal, and BB CPLD1/2 will be kept reset. But after write 40h with data 0x03, BB_CPLD_1/2_RST_L signal are low correctly, but CPLD1, CPLD2 isn't reset. 
-Reproduce Step: 
-1. Power on system, then switch to Primary SXP Uart by hotkey Ctrl+^ c. 
-2. Read MI CPLD register 40h by "cpld reg mi 0x40", check if it's 0x00. 
-3. Read BB CPLD1 register 00 by "cpld reg bb1 0x00", check if it's 0x25. 
-4. Write MI CPLD "cpld reg mi 0x40 0x01", read it again, check if it's 0x01. 
-5. Probe siganl BB_CPLD1_RST_L is low. 
-6. Read BB CPLD1 register 00 by "cpld reg bb1 0x00", chekc if it's still read out.</t>
-  </si>
-  <si>
-    <t>[Hardware] 
-Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
-Midplane - P/N: PBA001528A-A03, SN: JD37140690 
-BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
-[SW/FW Ver: Package 1] 
-Controller CPLD: V01.08 
-MI CPLD: V01.03 
-SXP: 0110[3257] 
-BMC: V005 
-Bios: V0101 
-BB CPLD: V01.02 
-SSM CPLD: V01.01 
-[Description] 
-As design spec definition, 1b means asserted, 0b means de-asserted, so for the loa active signals, 1b means signal high, 0b means signal low. 
-But 80[0:1] are 1b when CANISTER_A/B_PCIE_CLK_ACT_L are high, and 0b when CANISTER_A/B_PCIE_CLK_ACT_L are low. It's reversed. 
-Reprocude Step: 
-1. Power on system, and ctrl+D in Primary SXP debug port to let SXP into Bootloader. 
-2. Read 80h with Aardvark of CPLD 1. they are 0x03. 
-3. Probe CANISTER_A_PCIE_CLK_ACT_L is 3.3V(controller A inserted), CANISTER_B_PCIE_CLK_ACT_L is 2.4V(No controller B, 3.3V when B inserted) 
-4. Drive CANISTER_A_PCIE_CLK_ACT_L to Ground, read 80h again, it's 0x02. 
-5. Release CANISTER_A_PCIE_CLK_ACT_L, drive CANISTER_B_PCIE_CLK_ACT_L to Ground, read 80h again, it's 0x01.</t>
   </si>
   <si>
     <t>[Hardware] 
@@ -393,16 +335,84 @@
   <si>
     <t>13</t>
   </si>
+  <si>
+    <t>[Hardware] 
+Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
+Midplane - P/N: PBA001528A-A03, SN: JD37140690 
+BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
+[SW/FW Ver: Package 1] 
+Controller CPLD: V01.08 
+MI CPLD: V01.03 
+SXP: 0110[3257] 
+BMC: V005 
+Bios: V0101 
+BB CPLD: V01.02 
+SSM CPLD: V01.01 
+[Description] 
+As design spec definition, 1b means asserted, 0b means de-asserted, so for the loa active signals, 1b means signal high, 0b means signal low. 
+But 80[0:1] are 1b when CANISTER_A/B_PCIE_CLK_ACT_L are high, and 0b when CANISTER_A/B_PCIE_CLK_ACT_L are low. It's reversed. 
+Reprocude Step: 
+1. Power on system, and ctrl+D in Primary SXP debug port to let SXP into Bootloader. 
+2. Read 80h with Aardvark of CPLD 1. they are 0x03. 
+3. Probe CANISTER_A_PCIE_CLK_ACT_L is 3.3V(controller A inserted), CANISTER_B_PCIE_CLK_ACT_L is 2.4V(No controller B, 3.3V when B inserted) 
+4. Drive CANISTER_A_PCIE_CLK_ACT_L to Ground, read 80h again, it's 0x02. 
+5. Release CANISTER_A_PCIE_CLK_ACT_L, drive CANISTER_B_PCIE_CLK_ACT_L to Ground, read 80h again, it's 0x01.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix it in Baseboard_v0106, please verify</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Hardware] 
+Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
+Midplane - P/N: PBA001528A-A03, SN: JD37140690 
+BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
+[SW/FW Ver: Package 1] 
+Controller CPLD: V01.08 
+MI CPLD: V01.03 
+SXP: 0110[3257] 
+BMC: V005 
+Bios: V0101 
+BB CPLD: V01.02 
+SSM CPLD: V01.01 
+[Description] 
+MI CPLD register 40h BB_CPLD1/2_RST is required to drive BB_CPLD1/2_RST_L signal, and BB CPLD1/2 will be kept reset. But after write 40h with data 0x03, BB_CPLD_1/2_RST_L signal are low correctly, but CPLD1, CPLD2 isn't reset. 
+Reproduce Step: 
+1. Power on system, then switch to Primary SXP Uart by hotkey Ctrl+^ c. 
+2. Read MI CPLD register 40h by "cpld reg mi 0x40", check if it's 0x00. 
+3. Read BB CPLD1 register 00 by "cpld reg bb1 0x00", check if it's 0x25. 
+4. Write MI CPLD "cpld reg mi 0x40 0x01", read it again, check if it's 0x01. 
+5. Probe siganl BB_CPLD1_RST_L is low. 
+6. Read BB CPLD1 register 00 by "cpld reg bb1 0x00", chekc if it's still read out.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-0020797</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-0020567</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;EVT FW BB CPLD&gt; Register 80h 0b/1b is reversed to reflect the low active signal.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;EVT FW BB CPLD&gt; BB CPLD1/2 couldn't be reset by BB_CPLD1/2_RST_L signal.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -418,6 +428,21 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -450,7 +475,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
@@ -474,13 +499,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -970,7 +1004,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1012,7 +1046,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1044,9 +1078,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1078,6 +1113,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1253,272 +1289,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="12.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.125" style="5"/>
+    <col min="2" max="2" width="12.875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="5"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
     <col min="5" max="5" width="59" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="2.75" style="5" customWidth="1"/>
     <col min="7" max="7" width="55" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="8" max="16384" width="9.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="409.5">
+    <row r="1" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="297" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="351" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="229.5" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="351" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="351" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.5">
-      <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="9" spans="1:8" ht="364.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>22</v>
+      <c r="E9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="315">
-      <c r="A3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>24</v>
+      <c r="E10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="375">
-      <c r="A4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="255">
-      <c r="A5" s="5" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="375">
-      <c r="A7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="360">
-      <c r="A8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="375">
-      <c r="A9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="285">
-      <c r="A10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="409.5">
+    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="310.5" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="330">
-      <c r="A13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://c.na13.visual.force.com/apex/Actions_View?retURL=https%3A%2F%2Fc.na13.visual.force.com%2Fapex%2FProject_Defects%3FID%3Da04a000000Rtt0LAAR&amp;sfdc.override=1&amp;id=a02a000000LXvXfAAL"/>
     <hyperlink ref="B2" r:id="rId2" display="https://c.na13.visual.force.com/apex/Actions_View?retURL=https%3A%2F%2Fc.na13.visual.force.com%2Fapex%2FProject_Defects%3FID%3Da04a000000Rtt0LAAR&amp;sfdc.override=1&amp;id=a02a000000LgLy5AAF"/>
@@ -1540,25 +1583,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Baseboard_v0107 Fix below issue 1) D-0020586	0-None	Assigned	<EVT FW BB CPLD> Register A0h hasn't control SGPIO outputs enbale or disable. 2) D-0020539	0-None	Assigned	<EVT FW BB CPLD> DRIVE_xx_PWROK register couldn't reflect Drv[x]_PWR_EN_L signal state. 3) D-0020541	0-None	Assigned	<EVT FW BB CPLD> LED blink doesn't following the corresponding toggle rate. 4) D-0020538	0-None	Assigned	<EVT FW BB CPLD> Defalut value of some regsiters are not compliant with desgin spec
</commit_message>
<xml_diff>
--- a/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
+++ b/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>0-None</t>
   </si>
@@ -102,53 +102,8 @@
 BB CPLD: V01.02 
 SSM CPLD: V01.01 
 [Description] 
-As design spec V0.8, only when the register STATUS_BOARD_PRSENT asserted, SGPIO outputs are enabled to output ACTIVITY LED signals to SSM, otherwise SGPIO outputs always are disabled and no actionA0h STATUS_BOARD_PRSENT. But when 80h is 0x00, Activity LED still ON. 
-Reproduce Step: 
-1. Insert some HDDs, and power on system into OS. 
-2. Read regsiter A0h is 0x00 in Primary SXP debug port. 
-3. Use IO meter to trigger HDD activity. 
-3. Check the HDD Activity LED on the SSM Board. they are blink.</t>
-  </si>
-  <si>
-    <t>[Hardware] 
-Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
-Midplane - P/N: PBA001528A-A03, SN: JD37140690 
-BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
-[SW/FW Ver: Package 1] 
-Controller CPLD: V01.08 
-MI CPLD: V01.03 
-SXP: 0110[3257] 
-BMC: V005 
-Bios: V0101 
-BB CPLD: V01.02 
-SSM CPLD: V01.01 
-[Description] 
 1. Power OK register response different values even all the Drv[x]_PWR_EN_L signal are high. 
 2. Power OK value will not reflect the state of Drv[x]_PWR_EN_L even it changes.</t>
-  </si>
-  <si>
-    <t>[Hardware] 
-Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
-Midplane - P/N: PBA001528A-A03, SN: JD37140690 
-BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
-[SW/FW Ver: Package 1] 
-Controller CPLD: V01.08 
-MI CPLD: V01.03 
-SXP: 0110[3257] 
-BMC: V005 
-Bios: V0101 
-BB CPLD: V01.02 
-SSM CPLD: V01.01 
-[Description] 
-IFDET_BLUE_LED and PRSNT_AMBER_LED blink hasn't follow the toggle rate when rate is 0010, 0110 and 0111. 
-1. Toggle rate 0010 cause LED is ON 1 sec and OFF 1 sec which should be 500ms ON and 500ms OFF as design. 
-2. Toggle rate 0110 request "Repeated cycle of alternating between on and off at 4 Hz with a 50% duty cycle twice then on for a period of 500 milliseconds", but in fact it's 4 Hz with a 50% duty cycle twice then OFF in 500 ms. 
-3. Toggle rate 0111 request "Repeated cycle of alternating between on and off at 4 Hz with a 50% duty cycle twice then on for a period of 3.5 seconds", but infact it's 4 Hz with a 50% duty cycle twice then OFF in 3.5 seconds. 
-Please refer to the attached snapshot for 
-Reproduce Step: 
-1. Power on system, and ctrl+D in Primary SXP debug port to let SXP into Bootloader. 
-2. Wrtie register 0x70 with data 0x22, then check the HDD Fault and Identity LED is blink with ON and OFF simultaneously. 
-3. Probe DRV21_IFDET_BLUE_LED in HDD70 with oscilloscope to check the phase of the signal. the 50% duty cycle is 1s.</t>
   </si>
   <si>
     <t>[Hardware] 
@@ -401,6 +356,62 @@
   </si>
   <si>
     <t>&lt;EVT FW BB CPLD&gt; BB CPLD1/2 couldn't be reset by BB_CPLD1/2_RST_L signal.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Hardware] 
+Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
+Midplane - P/N: PBA001528A-A03, SN: JD37140690 
+BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
+[SW/FW Ver: Package 1] 
+Controller CPLD: V01.08 
+MI CPLD: V01.03 
+SXP: 0110[3257] 
+BMC: V005 
+Bios: V0101 
+BB CPLD: V01.02 
+SSM CPLD: V01.01 
+[Description] 
+As design spec V0.8, only when the register STATUS_BOARD_PRSENT asserted, SGPIO outputs are enabled to output ACTIVITY LED signals to SSM, otherwise SGPIO outputs always are disabled and no actionA0h STATUS_BOARD_PRSENT. But when 80h is 0x00, Activity LED still ON. 
+Reproduce Step: 
+1. Insert some HDDs, and power on system into OS. 
+2. Read regsiter A0h is 0x00 in Primary SXP debug port. 
+3. Use IO meter to trigger HDD activity. 
+3. Check the HDD Activity LED on the SSM Board. they are blink.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix it in Baseboard_v0107, please verify</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Hardware] 
+Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
+Midplane - P/N: PBA001528A-A03, SN: JD37140690 
+BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
+[SW/FW Ver: Package 1] 
+Controller CPLD: V01.08 
+MI CPLD: V01.03 
+SXP: 0110[3257] 
+BMC: V005 
+Bios: V0101 
+BB CPLD: V01.02 
+SSM CPLD: V01.01 
+[Description] 
+IFDET_BLUE_LED and PRSNT_AMBER_LED blink hasn't follow the toggle rate when rate is 0010, 0110 and 0111. 
+1. Toggle rate 0010 cause LED is ON 1 sec and OFF 1 sec which should be 500ms ON and 500ms OFF as design. 
+2. Toggle rate 0110 request "Repeated cycle of alternating between on and off at 4 Hz with a 50% duty cycle twice then on for a period of 500 milliseconds", but in fact it's 4 Hz with a 50% duty cycle twice then OFF in 500 ms. 
+3. Toggle rate 0111 request "Repeated cycle of alternating between on and off at 4 Hz with a 50% duty cycle twice then on for a period of 3.5 seconds", but infact it's 4 Hz with a 50% duty cycle twice then OFF in 3.5 seconds. 
+Please refer to the attached snapshot for 
+Reproduce Step: 
+1. Power on system, and ctrl+D in Primary SXP debug port to let SXP into Bootloader. 
+2. Wrtie register 0x70 with data 0x22, then check the HDD Fault and Identity LED is blink with ON and OFF simultaneously. 
+3. Probe DRV21_IFDET_BLUE_LED in HDD70 with oscilloscope to check the phase of the signal. the 50% duty cycle is 1s.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The driver type's default value is decide by hardware not CPLD, if "0" means SATA Driver, if "1" means PCIE Driver
+Fix it in Baseboard_v0107, please verify</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -475,7 +486,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
@@ -500,6 +511,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1292,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1305,15 +1319,16 @@
     <col min="5" max="5" width="59" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.75" style="5" customWidth="1"/>
     <col min="7" max="7" width="55" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="5"/>
+    <col min="8" max="8" width="41.625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1322,21 +1337,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -1345,18 +1360,18 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="297" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -1376,7 +1391,7 @@
     </row>
     <row r="4" spans="1:8" ht="351" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -1391,12 +1406,15 @@
         <v>5</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="229.5" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -1411,12 +1429,15 @@
         <v>7</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -1431,12 +1452,15 @@
         <v>9</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="351" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -1451,12 +1475,12 @@
         <v>11</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="351" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -1471,12 +1495,12 @@
         <v>13</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="364.5" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
@@ -1491,12 +1515,12 @@
         <v>15</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="324" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -1511,21 +1535,24 @@
         <v>17</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -1534,30 +1561,30 @@
         <v>1</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="310.5" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Baseboard_v0108 Fix below issue D-0020540	0-None	Assigned	<EVT FW BB CPLD> Protected Access Register couldn't be protected by protected key.
</commit_message>
<xml_diff>
--- a/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
+++ b/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>0-None</t>
   </si>
@@ -412,6 +412,10 @@
   <si>
     <t>The driver type's default value is decide by hardware not CPLD, if "0" means SATA Driver, if "1" means PCIE Driver
 Fix it in Baseboard_v0107, please verify</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix it in Baseboard_v0108, please verify</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1306,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1497,6 +1501,9 @@
       <c r="G8" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H8" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="364.5" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
@@ -1518,7 +1525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="324" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Status_v0102 Fix below issue D-0020587	0-None	Assigned	<EVT FW SSM CPLD> Most pattern of LED blinking don't match the corresponding toggle rate. D-0020588	0-None	Proposed Fix	<EVT FW SSM CPLD> Mapping of Register 11h,13h and LEDs are incorrect.
</commit_message>
<xml_diff>
--- a/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
+++ b/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>0-None</t>
   </si>
@@ -104,27 +104,6 @@
 [Description] 
 1. Power OK register response different values even all the Drv[x]_PWR_EN_L signal are high. 
 2. Power OK value will not reflect the state of Drv[x]_PWR_EN_L even it changes.</t>
-  </si>
-  <si>
-    <t>[Hardware] 
-Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
-Midplane - P/N: PBA001528A-A03, SN: JD37140690 
-BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
-[SW/FW Ver: Package 1] 
-Controller CPLD: V01.08 
-MI CPLD: V01.03 
-SXP: 0110[3257] 
-BMC: V005 
-Bios: V0101 
-BB CPLD: V01.02 
-SSM CPLD: V01.01 
-[Description] 
-As design spec, register read operations support Sequential read in BB CPLD and SSM CPLD. But it couldn't take effect. 
-Reproduce steps: 
-1. Adapt Sequential register read to read BB CPLD 6 registers (0x06 through 0x05) via Aardvark GUI. 
-2. Check the responsed data 20 FF FF FF FF FF. 
-3. Random register read BB CPLD register 0x00, 0x01, 0x02, 0x03, 0x04, 0x05. 
-4. Check the responsed data each operation, they are 20, 14, 01, 02, 00, C9</t>
   </si>
   <si>
     <t>[Hardware] 
@@ -416,6 +395,32 @@
   </si>
   <si>
     <t>Fix it in Baseboard_v0108, please verify</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Hardware] 
+Controller - P/N: PBA001540B-B03 EVT, SN: JD46140014 
+Midplane - P/N: PBA001528A-A03, SN: JD37140690 
+BB - P/N: PBA001529A-A04 EVT, SN: JD40140030 
+[SW/FW Ver: Package 1] 
+Controller CPLD: V01.08 
+MI CPLD: V01.03 
+SXP: 0110[3257] 
+BMC: V005 
+Bios: V0101 
+BB CPLD: V01.02 
+SSM CPLD: V01.01 
+[Description] 
+As design spec, register read operations support Sequential read in BB CPLD and SSM CPLD. But it couldn't take effect. 
+Reproduce steps: 
+1. Adapt Sequential register read to read BB CPLD 6 registers (0x06 through 0x05) via Aardvark GUI. 
+2. Check the responsed data 20 FF FF FF FF FF. 
+3. Random register read BB CPLD register 0x00, 0x01, 0x02, 0x03, 0x04, 0x05. 
+4. Check the responsed data each operation, they are 20, 14, 01, 02, 00, C9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix it in Status_v0102</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1310,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1329,10 +1334,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1341,21 +1346,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -1364,18 +1369,18 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="297" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -1395,7 +1400,7 @@
     </row>
     <row r="4" spans="1:8" ht="351" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -1410,15 +1415,15 @@
         <v>5</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="229.5" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -1436,12 +1441,12 @@
         <v>19</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -1456,15 +1461,15 @@
         <v>9</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="351" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -1479,12 +1484,12 @@
         <v>11</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="351" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -1499,15 +1504,15 @@
         <v>13</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="364.5" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
@@ -1522,12 +1527,12 @@
         <v>15</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -1542,24 +1547,24 @@
         <v>17</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -1568,30 +1573,36 @@
         <v>1</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="310.5" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="G13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Baseboard_v0109 Fix below issue D-0020537	0-None	Assigned	<EVT FW BB/SSM CPLD> Sequential read doesn't take effect in BB CPLD and SSM CPLD D-0020566	0-None	Assigned	<EVT FW BB CPLD> HDD present status change hasn't trigger Alert
</commit_message>
<xml_diff>
--- a/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
+++ b/Baseboard/Release/WC_CPLD_salesforce_bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>0-None</t>
   </si>
@@ -421,6 +421,10 @@
   </si>
   <si>
     <t>Fix it in Status_v0102</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix it in Baseboard_v0109, please verify</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1315,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1486,6 +1490,9 @@
       <c r="G7" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="H7" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="351" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
@@ -1528,6 +1535,9 @@
       </c>
       <c r="G9" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.15">

</xml_diff>